<commit_message>
Filter path list from bread crumb data.
</commit_message>
<xml_diff>
--- a/test-data/BreadCrumbData.xlsx
+++ b/test-data/BreadCrumbData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/learnb/git/digiplat-qa/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC32CFF0-A42B-C34A-8AAC-68709F6FBA67}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDEE3EB2-1D4A-EB4A-BFF2-116185C95154}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5460" windowWidth="28040" windowHeight="17440" xr2:uid="{150E7FB9-AAC7-684F-9B42-02331F762CE7}"/>
+    <workbookView xWindow="57380" yWindow="3560" windowWidth="28040" windowHeight="17440" xr2:uid="{150E7FB9-AAC7-684F-9B42-02331F762CE7}"/>
   </bookViews>
   <sheets>
     <sheet name="SimplePageList" sheetId="1" r:id="rId1"/>
@@ -30,12 +30,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>path</t>
   </si>
   <si>
     <t>about-cancer/coping/feelings</t>
+  </si>
+  <si>
+    <t>/grants-training/apply-grant/development</t>
+  </si>
+  <si>
+    <t>/news-events/press-releases/2018/cll-ibrutinib-trial</t>
+  </si>
+  <si>
+    <t>/news-events/cancer-currents-blog</t>
+  </si>
+  <si>
+    <t>news-events/cancer-currents-blog/2018/cancer-moonshot-planning-to-research</t>
+  </si>
+  <si>
+    <t>news-events/press-releases/2015/ilc-2015</t>
+  </si>
+  <si>
+    <t>/about-nci/budget/congressional-justification</t>
+  </si>
+  <si>
+    <t>/about-nci/budget/about-annual-plan</t>
+  </si>
+  <si>
+    <t>about-nci/budget/fact-book/historical-trends</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>Article</t>
+  </si>
+  <si>
+    <t>Press Release</t>
+  </si>
+  <si>
+    <t>Blog Series</t>
+  </si>
+  <si>
+    <t>Blog Post</t>
+  </si>
+  <si>
+    <t>General</t>
   </si>
 </sst>
 </file>
@@ -71,8 +113,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,25 +430,95 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41E50E58-C20E-6840-B475-2B9A8D9E132C}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
+    <col min="1" max="1" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>